<commit_message>
Fixed Import from MongoDB button
</commit_message>
<xml_diff>
--- a/Excel/Manufacturers.xlsx
+++ b/Excel/Manufacturers.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,7 +353,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -364,7 +364,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>